<commit_message>
Not sure if the data changes because the file name is new or if there are actual changes, or how to interrogate that with git.
</commit_message>
<xml_diff>
--- a/data/fromR/top_ten_threatened.xlsx
+++ b/data/fromR/top_ten_threatened.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/Rstudio_Git/threatRF/data/fromR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79526D72-D258-464E-8BDE-C7000E1BB63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{33BFBB55-F899-EB49-8A93-FE0E33CD6FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="30240" yWindow="900" windowWidth="19940" windowHeight="19240"/>
   </bookViews>
   <sheets>
     <sheet name="top_ten_threatened" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>lepidoptera</t>
   </si>
@@ -185,9 +185,6 @@
   </si>
   <si>
     <t>VA, NC S1 DE S2</t>
-  </si>
-  <si>
-    <t>CHECK ME</t>
   </si>
   <si>
     <t>NC, DE S3</t>
@@ -1068,7 +1065,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,8 +1318,8 @@
       <c r="D13" s="4">
         <v>0.97199999999999998</v>
       </c>
-      <c r="E13" t="s">
-        <v>55</v>
+      <c r="E13" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="F13" t="s">
         <v>48</v>
@@ -1342,10 +1339,10 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
         <v>56</v>
-      </c>
-      <c r="F14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1362,10 +1359,10 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,7 +1379,7 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
         <v>48</v>
@@ -1402,7 +1399,7 @@
         <v>0.96</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1419,7 +1416,7 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1436,7 +1433,7 @@
         <v>0.95199999999999996</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
         <v>48</v>
@@ -1456,7 +1453,7 @@
         <v>0.95199999999999996</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1473,10 +1470,10 @@
         <v>0.95</v>
       </c>
       <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" t="s">
         <v>62</v>
-      </c>
-      <c r="F21" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>